<commit_message>
jan 28 update 2
</commit_message>
<xml_diff>
--- a/Data/SurveyTrackingCalendar.xlsx
+++ b/Data/SurveyTrackingCalendar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abautist/Dropbox (University of Oregon)/RAPID-EC/Data Management R3/EE_R3 Question Bank/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF2F4C8-E162-4D4B-8D8D-ADE308BB98B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B597703-F1F2-934B-8624-04EF55A861D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35200" yWindow="4000" windowWidth="26440" windowHeight="15040" xr2:uid="{C19A8553-E830-DE48-8F7A-F28455544AB6}"/>
+    <workbookView xWindow="35160" yWindow="3940" windowWidth="26440" windowHeight="15040" xr2:uid="{C19A8553-E830-DE48-8F7A-F28455544AB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="107">
   <si>
     <t>Survey</t>
   </si>
@@ -33,9 +33,6 @@
     <t xml:space="preserve">Date Range </t>
   </si>
   <si>
-    <t>Special Topic Implemented</t>
-  </si>
-  <si>
     <t>Baseline</t>
   </si>
   <si>
@@ -180,15 +177,6 @@
     <t>Child Care - Alliance For Early Success</t>
   </si>
   <si>
-    <t xml:space="preserve">Child Care Reopening Questions </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social Support, Material Hardship, Unemployment Benefits </t>
-  </si>
-  <si>
-    <t>Social Support, Material Hardship,  Unemployment Benefits, School Reopening Questions, RISER Questions</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -204,9 +192,6 @@
     <t>Sept 8 - Sept 10</t>
   </si>
   <si>
-    <t xml:space="preserve">Social Support, Material Hardship, Unemployment Benefits, School Reopening Questions, RISER Questions </t>
-  </si>
-  <si>
     <t>Survey 24</t>
   </si>
   <si>
@@ -219,9 +204,6 @@
     <t>Sept 21 - Sept 24</t>
   </si>
   <si>
-    <t xml:space="preserve">Material Hardship, Unemployment Benefits, RISER Questions, Family Routine Questions </t>
-  </si>
-  <si>
     <t xml:space="preserve">Survey 26 </t>
   </si>
   <si>
@@ -252,25 +234,170 @@
     <t xml:space="preserve">Oct 26 - Oct 29 </t>
   </si>
   <si>
-    <t>Food insecurity, Material Hardship,  Unemployment Benefits,  RISER, Family Routine</t>
-  </si>
-  <si>
-    <t>RISER Questions, Attitudes towards COVID Vaccine, Family Conflict</t>
-  </si>
-  <si>
     <t>Survey 31</t>
   </si>
   <si>
     <t>Nov 03 - Nov 05</t>
   </si>
   <si>
-    <t>RISER Questions, Attitudes towards COVID Vaccine, Material Hardship, Food Insecurity</t>
-  </si>
-  <si>
     <t>Survey 32</t>
   </si>
   <si>
     <t>Nov 17 - Nov 19</t>
+  </si>
+  <si>
+    <t>Modules / Special Topic Implemented</t>
+  </si>
+  <si>
+    <t>Survey 33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Survey 34 </t>
+  </si>
+  <si>
+    <t>Survey 35</t>
+  </si>
+  <si>
+    <t>Survey 36</t>
+  </si>
+  <si>
+    <t>Survey 37</t>
+  </si>
+  <si>
+    <t>Survey 38</t>
+  </si>
+  <si>
+    <t>Survey 39</t>
+  </si>
+  <si>
+    <t>Survey 40</t>
+  </si>
+  <si>
+    <t>Survey 41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nov 17 - Nov 19 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nov 22 - Nov 26 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dec 1 - Dec 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dec 7 - Dec 10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dec 15 - Dec 17 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dec 21 - Dec 24 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan 5 - Jan 7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan 11 - Jan 14 </t>
+  </si>
+  <si>
+    <t>Jan 20 - Jan 22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social Support
+Material Hardship 
+Unemployment Benefits </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social Support
+Material Hardship
+Unemployment Benefits
+School Reopening 
+RISER </t>
+  </si>
+  <si>
+    <t>Child Care Reopening</t>
+  </si>
+  <si>
+    <t>Social Support
+Material Hardship
+Unemployment Benefits
+School Reopening
+RISER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Material Hardship
+Unemployment Benefits
+RISER Questions
+Family Routine Questions </t>
+  </si>
+  <si>
+    <t>Food insecurity
+Material Hardship
+Unemployment Benefits
+RISER, Family Routine</t>
+  </si>
+  <si>
+    <t>RISER Questions
+Attitudes towards COVID Vaccine
+Family Conflict</t>
+  </si>
+  <si>
+    <t>RISER Questions
+Vaccines 
+Material Hardship
+Food Insecurity</t>
+  </si>
+  <si>
+    <t>Remote Learning
+Vaccines
+Holiday Plans
+RISER
+Workforce 
+Remote Work
+Food Insecurity
+Material Hardship</t>
+  </si>
+  <si>
+    <t>School Mobility
+Healthcare 
+Vaccines
+Social Support
+RISER
+Employment
+Unemployment 
+Food Insecurity
+Diapers</t>
+  </si>
+  <si>
+    <t>Grandparents 
+School Mobility 
+Remote Learning 
+RISER 
+Workforce 
+Remote Work 
+Other Hardship</t>
+  </si>
+  <si>
+    <t>Remote Learning 
+Healthcare
+RISER Module
+Employment
+Unemployment
+Food Insecurity
+Other Hardship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaccines
+Workforce
+Remote Work
+Food Insecurity
+Other Hardship </t>
+  </si>
+  <si>
+    <t>Survey 42</t>
+  </si>
+  <si>
+    <t>Jan 25 - Jan 28</t>
   </si>
 </sst>
 </file>
@@ -625,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D45FA6A-9962-6745-879A-BF18C9670907}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -646,458 +773,583 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="119" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="153" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="136" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>21</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B26" t="s">
         <v>42</v>
       </c>
-      <c r="C18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" t="s">
-        <v>58</v>
-      </c>
-      <c r="D24" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>64</v>
+      <c r="C26" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>40</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="B29" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="D29" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>73</v>
+        <v>38</v>
+      </c>
+      <c r="C30" t="s">
+        <v>50</v>
       </c>
       <c r="D30" t="s">
-        <v>54</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="C31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="D31" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>36</v>
+      </c>
+      <c r="C32" t="s">
+        <v>50</v>
       </c>
       <c r="D32" t="s">
-        <v>54</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="B33" t="s">
-        <v>81</v>
+        <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="D33" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>